<commit_message>
realizando roteiro no dashboard e boletins detalhados
</commit_message>
<xml_diff>
--- a/Boletim_de_Medição_-_Roteiro_de_Testes.xlsx
+++ b/Boletim_de_Medição_-_Roteiro_de_Testes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\source\LojaInterativa\taesa-boletimmedicao-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D1C188-0711-4B72-A3AF-20303DEDBE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9D2B48-04AE-4665-A282-DD4D703099D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="966" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="966" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configurações" sheetId="1" r:id="rId1"/>
     <sheet name="Dashboard" sheetId="2" r:id="rId2"/>
+    <sheet name="Boletim Detalhado" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="202">
   <si>
     <t xml:space="preserve">                                                                                                           Boletim de Medição - Roteiro de Testes</t>
   </si>
@@ -2359,6 +2360,484 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Ao clicar no botão a ação correspondente deve ser realizada corretamente.</t>
+    </r>
+  </si>
+  <si>
+    <t>Tab dados</t>
+  </si>
+  <si>
+    <t>Tab boletim</t>
+  </si>
+  <si>
+    <t>Tab comentários</t>
+  </si>
+  <si>
+    <t>Tab CAF</t>
+  </si>
+  <si>
+    <t>Tab notas fiscais</t>
+  </si>
+  <si>
+    <t>Tab relatório financeiro</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Teste de rota do tab "Dados": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ao clicar na tab "Dados". O sistema deve navegar para tela "Dados". </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Teste de rota do tab "Comentários": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ao clicar na tab "Comentários". O sistema deve navegar para tela "Comentários". </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Teste de rota do tab "CAF": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ao clicar na tab "CAF". O sistema deve navegar para tela "CAF". </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Teste de rota do tab "Notas fiscais": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ao clicar na tab "Notas fiscais". O sistema deve navegar para tela "Notas fiscais". </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Teste de rota do tab "Relatório financeiro": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ao clicar na tab "Relatório financeiro". O sistema deve navegar para tela "Relatório financeiro". </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de estado ativo/passivo:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Quando navegar para esta "tab dados" esta tab deve ser realçada e indicada como a página ativa atualmente.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de estado ativo/passivo:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Quando navegar para esta "tab comentários" esta tab deve ser realçada e indicada como a página ativa atualmente.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de estado ativo/passivo:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Quando navegar para esta "tab caf" esta tab deve ser realçada e indicada como a página ativa atualmente.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de estado ativo/passivo:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Quando navegar para esta "tab notas fiscais" esta tab deve ser realçada e indicada como a página ativa atualmente.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de estado ativo/passivo:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Quando navegar para esta "tab relatório financeiro" esta tab deve ser realçada e indicada como a página ativa atualmente.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Teste de exibição do status: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>O status de cada boletim e seus passos correspondentes devem ser exibidos corretamente.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de atualização do status:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> O status de cada boletim deve ser atualizado corretamente conforme os passos são concluídos.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de responsividade:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> A "tab dados" deve ser exibido corretamente em diferentes tamanhos de tela.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de responsividade:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> A "tab comentários" deve ser exibido corretamente em diferentes tamanhos de tela.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de responsividade:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> A "tab caf" deve ser exibido corretamente em diferentes tamanhos de tela.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de responsividade:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> A "tab notas fiscais" deve ser exibido corretamente em diferentes tamanhos de tela.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de responsividade:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> A "tab relatório financeiro" deve ser exibido corretamente em diferentes tamanhos de tela.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de exibição dos dados:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Todos os dados relevantes do boletim devem ser exibidos corretamente.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Teste de correspondência dos dados: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cada dado exibido deve corresponder à informação correta do boletim.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de exibição dos responsáveis:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Os responsáveis relevantes para o boletim devem ser exibidos corretamente.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de correspondência dos responsáveis:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Cada responsável exibido deve corresponder à pessoa correta associada ao boletim.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de exibição do log de ações:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Todas as ações relevantes para o boletim devem ser exibidas corretamente no log de ações.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Teste de atualização do log de ações:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> O log de ações deve ser atualizado corretamente conforme as ações são realizadas.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Teste de clique no botão "Registrar avanço": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ao clicar no registrar avanço os dados devem ser registrados.</t>
     </r>
   </si>
 </sst>
@@ -2557,7 +3036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2622,6 +3101,7 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2680,16 +3160,16 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -2985,8 +3465,8 @@
   </sheetPr>
   <dimension ref="A1:G1164"/>
   <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView topLeftCell="A88" zoomScale="80" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102:D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2997,32 +3477,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="47" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30">
+      <c r="A3" s="31">
         <v>1</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="19">
@@ -3036,8 +3516,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30"/>
-      <c r="B4" s="41"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="19">
         <v>2</v>
       </c>
@@ -3049,8 +3529,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
-      <c r="B5" s="41"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="19">
         <v>3</v>
       </c>
@@ -3062,8 +3542,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
-      <c r="B6" s="41"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="19">
         <v>4</v>
       </c>
@@ -3075,8 +3555,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
-      <c r="B7" s="41"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="19">
         <v>5</v>
       </c>
@@ -3088,10 +3568,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="40">
+      <c r="A8" s="41">
         <v>2</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="44" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="3">
@@ -3105,8 +3585,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="40"/>
-      <c r="B9" s="43"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="3">
         <v>2</v>
       </c>
@@ -3118,10 +3598,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40">
+      <c r="A10" s="41">
         <v>3</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="42" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="19">
@@ -3135,8 +3615,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="19">
         <v>2</v>
       </c>
@@ -3148,8 +3628,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="19">
         <v>3</v>
       </c>
@@ -3161,8 +3641,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="40"/>
-      <c r="B13" s="41"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="19">
         <v>4</v>
       </c>
@@ -3174,8 +3654,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
-      <c r="B14" s="41"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="19">
         <v>5</v>
       </c>
@@ -3187,8 +3667,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
-      <c r="B15" s="41"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="19">
         <v>6</v>
       </c>
@@ -3200,8 +3680,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
-      <c r="B16" s="41"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="19">
         <v>7</v>
       </c>
@@ -3213,8 +3693,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="40"/>
-      <c r="B17" s="41"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="19">
         <v>8</v>
       </c>
@@ -3226,8 +3706,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="40"/>
-      <c r="B18" s="41"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="19">
         <v>9</v>
       </c>
@@ -3239,10 +3719,10 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="30">
+      <c r="A19" s="31">
         <v>4</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="40" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="6">
@@ -3256,8 +3736,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="30"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="6">
         <v>2</v>
       </c>
@@ -3269,8 +3749,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="30"/>
-      <c r="B21" s="39"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="40"/>
       <c r="C21" s="6">
         <v>3</v>
       </c>
@@ -3282,8 +3762,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="30"/>
-      <c r="B22" s="39"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="6">
         <v>4</v>
       </c>
@@ -3295,8 +3775,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="30"/>
-      <c r="B23" s="39"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="40"/>
       <c r="C23" s="6">
         <v>5</v>
       </c>
@@ -3308,8 +3788,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="30"/>
-      <c r="B24" s="39"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="40"/>
       <c r="C24" s="6">
         <v>6</v>
       </c>
@@ -3321,8 +3801,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="30"/>
-      <c r="B25" s="39"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="6">
         <v>7</v>
       </c>
@@ -3334,8 +3814,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="30"/>
-      <c r="B26" s="39"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="40"/>
       <c r="C26" s="6">
         <v>7</v>
       </c>
@@ -3347,8 +3827,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="30"/>
-      <c r="B27" s="39"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="6">
         <v>8</v>
       </c>
@@ -3360,8 +3840,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="30"/>
-      <c r="B28" s="39"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="6">
         <v>9</v>
       </c>
@@ -3373,10 +3853,10 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="40">
+      <c r="A29" s="41">
         <v>5</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="43" t="s">
         <v>35</v>
       </c>
       <c r="C29" s="19">
@@ -3390,8 +3870,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="40"/>
-      <c r="B30" s="42"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="19">
         <v>2</v>
       </c>
@@ -3403,8 +3883,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="40"/>
-      <c r="B31" s="42"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="43"/>
       <c r="C31" s="19">
         <v>3</v>
       </c>
@@ -3416,8 +3896,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="40"/>
-      <c r="B32" s="42"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="43"/>
       <c r="C32" s="19">
         <v>4</v>
       </c>
@@ -3429,8 +3909,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="40"/>
-      <c r="B33" s="42"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="43"/>
       <c r="C33" s="19">
         <v>5</v>
       </c>
@@ -3442,8 +3922,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="40"/>
-      <c r="B34" s="42"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="43"/>
       <c r="C34" s="19">
         <v>6</v>
       </c>
@@ -3455,8 +3935,8 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="40"/>
-      <c r="B35" s="42"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="43"/>
       <c r="C35" s="19">
         <v>7</v>
       </c>
@@ -3468,10 +3948,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="30">
-        <v>6</v>
-      </c>
-      <c r="B36" s="29" t="s">
+      <c r="A36" s="31">
+        <v>6</v>
+      </c>
+      <c r="B36" s="30" t="s">
         <v>43</v>
       </c>
       <c r="C36" s="6">
@@ -3485,8 +3965,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="30"/>
-      <c r="B37" s="29"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="6">
         <v>2</v>
       </c>
@@ -3498,8 +3978,8 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="30"/>
-      <c r="B38" s="29"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="30"/>
       <c r="C38" s="6">
         <v>3</v>
       </c>
@@ -3511,8 +3991,8 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="30"/>
-      <c r="B39" s="29"/>
+      <c r="A39" s="31"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="6">
         <v>4</v>
       </c>
@@ -3524,8 +4004,8 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="30"/>
-      <c r="B40" s="29"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="6">
         <v>5</v>
       </c>
@@ -3537,8 +4017,8 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="30"/>
-      <c r="B41" s="29"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="6">
         <v>6</v>
       </c>
@@ -3551,8 +4031,8 @@
       <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="30"/>
-      <c r="B42" s="29"/>
+      <c r="A42" s="31"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="6">
         <v>7</v>
       </c>
@@ -3565,10 +4045,10 @@
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="40">
+      <c r="A43" s="41">
         <v>7</v>
       </c>
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="42" t="s">
         <v>49</v>
       </c>
       <c r="C43" s="19">
@@ -3582,8 +4062,8 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="40"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="19">
         <v>2</v>
       </c>
@@ -3595,8 +4075,8 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="40"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="19">
         <v>3</v>
       </c>
@@ -3608,8 +4088,8 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="40"/>
-      <c r="B46" s="41"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="42"/>
       <c r="C46" s="19">
         <v>4</v>
       </c>
@@ -3621,8 +4101,8 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="40"/>
-      <c r="B47" s="41"/>
+      <c r="A47" s="41"/>
+      <c r="B47" s="42"/>
       <c r="C47" s="19">
         <v>5</v>
       </c>
@@ -3634,8 +4114,8 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="40"/>
-      <c r="B48" s="41"/>
+      <c r="A48" s="41"/>
+      <c r="B48" s="42"/>
       <c r="C48" s="19">
         <v>6</v>
       </c>
@@ -3647,8 +4127,8 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="40"/>
-      <c r="B49" s="41"/>
+      <c r="A49" s="41"/>
+      <c r="B49" s="42"/>
       <c r="C49" s="19">
         <v>7</v>
       </c>
@@ -3660,8 +4140,8 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="40"/>
-      <c r="B50" s="41"/>
+      <c r="A50" s="41"/>
+      <c r="B50" s="42"/>
       <c r="C50" s="19">
         <v>8</v>
       </c>
@@ -3673,10 +4153,10 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="30">
+      <c r="A51" s="31">
         <v>8</v>
       </c>
-      <c r="B51" s="39" t="s">
+      <c r="B51" s="40" t="s">
         <v>56</v>
       </c>
       <c r="C51" s="6">
@@ -3690,8 +4170,8 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="30"/>
-      <c r="B52" s="39"/>
+      <c r="A52" s="31"/>
+      <c r="B52" s="40"/>
       <c r="C52" s="6">
         <v>2</v>
       </c>
@@ -3703,8 +4183,8 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="30"/>
-      <c r="B53" s="39"/>
+      <c r="A53" s="31"/>
+      <c r="B53" s="40"/>
       <c r="C53" s="6">
         <v>3</v>
       </c>
@@ -3716,8 +4196,8 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="30"/>
-      <c r="B54" s="39"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="40"/>
       <c r="C54" s="6">
         <v>4</v>
       </c>
@@ -3729,8 +4209,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="30"/>
-      <c r="B55" s="39"/>
+      <c r="A55" s="31"/>
+      <c r="B55" s="40"/>
       <c r="C55" s="6">
         <v>5</v>
       </c>
@@ -3742,8 +4222,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="30"/>
-      <c r="B56" s="39"/>
+      <c r="A56" s="31"/>
+      <c r="B56" s="40"/>
       <c r="C56" s="6">
         <v>6</v>
       </c>
@@ -3755,8 +4235,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="30"/>
-      <c r="B57" s="39"/>
+      <c r="A57" s="31"/>
+      <c r="B57" s="40"/>
       <c r="C57" s="6">
         <v>7</v>
       </c>
@@ -3768,8 +4248,8 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="30"/>
-      <c r="B58" s="39"/>
+      <c r="A58" s="31"/>
+      <c r="B58" s="40"/>
       <c r="C58" s="6">
         <v>8</v>
       </c>
@@ -3781,10 +4261,10 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="40">
+      <c r="A59" s="41">
         <v>9</v>
       </c>
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="42" t="s">
         <v>65</v>
       </c>
       <c r="C59" s="19">
@@ -3798,8 +4278,8 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="40"/>
-      <c r="B60" s="41"/>
+      <c r="A60" s="41"/>
+      <c r="B60" s="42"/>
       <c r="C60" s="19">
         <v>2</v>
       </c>
@@ -3811,8 +4291,8 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="40"/>
-      <c r="B61" s="41"/>
+      <c r="A61" s="41"/>
+      <c r="B61" s="42"/>
       <c r="C61" s="19">
         <v>3</v>
       </c>
@@ -3824,8 +4304,8 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="40"/>
-      <c r="B62" s="41"/>
+      <c r="A62" s="41"/>
+      <c r="B62" s="42"/>
       <c r="C62" s="19">
         <v>4</v>
       </c>
@@ -3837,8 +4317,8 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="40"/>
-      <c r="B63" s="41"/>
+      <c r="A63" s="41"/>
+      <c r="B63" s="42"/>
       <c r="C63" s="19">
         <v>5</v>
       </c>
@@ -3850,8 +4330,8 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="40"/>
-      <c r="B64" s="41"/>
+      <c r="A64" s="41"/>
+      <c r="B64" s="42"/>
       <c r="C64" s="19">
         <v>6</v>
       </c>
@@ -3863,8 +4343,8 @@
       </c>
     </row>
     <row r="65" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="40"/>
-      <c r="B65" s="41"/>
+      <c r="A65" s="41"/>
+      <c r="B65" s="42"/>
       <c r="C65" s="19">
         <v>7</v>
       </c>
@@ -3876,8 +4356,8 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="40"/>
-      <c r="B66" s="41"/>
+      <c r="A66" s="41"/>
+      <c r="B66" s="42"/>
       <c r="C66" s="19">
         <v>8</v>
       </c>
@@ -3889,8 +4369,8 @@
       </c>
     </row>
     <row r="67" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="40"/>
-      <c r="B67" s="41"/>
+      <c r="A67" s="41"/>
+      <c r="B67" s="42"/>
       <c r="C67" s="19">
         <v>9</v>
       </c>
@@ -3902,10 +4382,10 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="30">
+      <c r="A68" s="31">
         <v>10</v>
       </c>
-      <c r="B68" s="34" t="s">
+      <c r="B68" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C68" s="5">
@@ -3919,8 +4399,8 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="30"/>
-      <c r="B69" s="34"/>
+      <c r="A69" s="31"/>
+      <c r="B69" s="35"/>
       <c r="C69" s="5">
         <v>2</v>
       </c>
@@ -3932,8 +4412,8 @@
       </c>
     </row>
     <row r="70" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="30"/>
-      <c r="B70" s="34"/>
+      <c r="A70" s="31"/>
+      <c r="B70" s="35"/>
       <c r="C70" s="5">
         <v>3</v>
       </c>
@@ -3945,8 +4425,8 @@
       </c>
     </row>
     <row r="71" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="30"/>
-      <c r="B71" s="34"/>
+      <c r="A71" s="31"/>
+      <c r="B71" s="35"/>
       <c r="C71" s="5">
         <v>4</v>
       </c>
@@ -3958,8 +4438,8 @@
       </c>
     </row>
     <row r="72" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="30"/>
-      <c r="B72" s="34"/>
+      <c r="A72" s="31"/>
+      <c r="B72" s="35"/>
       <c r="C72" s="5">
         <v>5</v>
       </c>
@@ -3971,8 +4451,8 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="30"/>
-      <c r="B73" s="34"/>
+      <c r="A73" s="31"/>
+      <c r="B73" s="35"/>
       <c r="C73" s="5">
         <v>6</v>
       </c>
@@ -3984,8 +4464,8 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="30"/>
-      <c r="B74" s="34"/>
+      <c r="A74" s="31"/>
+      <c r="B74" s="35"/>
       <c r="C74" s="5">
         <v>7</v>
       </c>
@@ -3997,8 +4477,8 @@
       </c>
     </row>
     <row r="75" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="30"/>
-      <c r="B75" s="34"/>
+      <c r="A75" s="31"/>
+      <c r="B75" s="35"/>
       <c r="C75" s="5">
         <v>8</v>
       </c>
@@ -4010,10 +4490,10 @@
       </c>
     </row>
     <row r="76" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="36">
+      <c r="A76" s="37">
         <v>11</v>
       </c>
-      <c r="B76" s="32" t="s">
+      <c r="B76" s="33" t="s">
         <v>77</v>
       </c>
       <c r="C76" s="19">
@@ -4027,8 +4507,8 @@
       </c>
     </row>
     <row r="77" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="36"/>
-      <c r="B77" s="32"/>
+      <c r="A77" s="37"/>
+      <c r="B77" s="33"/>
       <c r="C77" s="19">
         <v>2</v>
       </c>
@@ -4040,8 +4520,8 @@
       </c>
     </row>
     <row r="78" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="36"/>
-      <c r="B78" s="32"/>
+      <c r="A78" s="37"/>
+      <c r="B78" s="33"/>
       <c r="C78" s="19">
         <v>3</v>
       </c>
@@ -4053,8 +4533,8 @@
       </c>
     </row>
     <row r="79" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="36"/>
-      <c r="B79" s="32"/>
+      <c r="A79" s="37"/>
+      <c r="B79" s="33"/>
       <c r="C79" s="19">
         <v>4</v>
       </c>
@@ -4066,8 +4546,8 @@
       </c>
     </row>
     <row r="80" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="36"/>
-      <c r="B80" s="32"/>
+      <c r="A80" s="37"/>
+      <c r="B80" s="33"/>
       <c r="C80" s="19">
         <v>5</v>
       </c>
@@ -4079,8 +4559,8 @@
       </c>
     </row>
     <row r="81" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="36"/>
-      <c r="B81" s="32"/>
+      <c r="A81" s="37"/>
+      <c r="B81" s="33"/>
       <c r="C81" s="19">
         <v>6</v>
       </c>
@@ -4092,8 +4572,8 @@
       </c>
     </row>
     <row r="82" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="36"/>
-      <c r="B82" s="32"/>
+      <c r="A82" s="37"/>
+      <c r="B82" s="33"/>
       <c r="C82" s="19">
         <v>7</v>
       </c>
@@ -4105,8 +4585,8 @@
       </c>
     </row>
     <row r="83" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="36"/>
-      <c r="B83" s="32"/>
+      <c r="A83" s="37"/>
+      <c r="B83" s="33"/>
       <c r="C83" s="19">
         <v>8</v>
       </c>
@@ -4118,8 +4598,8 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="36"/>
-      <c r="B84" s="32"/>
+      <c r="A84" s="37"/>
+      <c r="B84" s="33"/>
       <c r="C84" s="19">
         <v>9</v>
       </c>
@@ -4131,8 +4611,8 @@
       </c>
     </row>
     <row r="85" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="36"/>
-      <c r="B85" s="32"/>
+      <c r="A85" s="37"/>
+      <c r="B85" s="33"/>
       <c r="C85" s="19">
         <v>10</v>
       </c>
@@ -4144,8 +4624,8 @@
       </c>
     </row>
     <row r="86" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="36"/>
-      <c r="B86" s="32"/>
+      <c r="A86" s="37"/>
+      <c r="B86" s="33"/>
       <c r="C86" s="19">
         <v>12</v>
       </c>
@@ -4157,8 +4637,8 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="36"/>
-      <c r="B87" s="32"/>
+      <c r="A87" s="37"/>
+      <c r="B87" s="33"/>
       <c r="C87" s="19">
         <v>12</v>
       </c>
@@ -4170,8 +4650,8 @@
       </c>
     </row>
     <row r="88" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="36"/>
-      <c r="B88" s="32"/>
+      <c r="A88" s="37"/>
+      <c r="B88" s="33"/>
       <c r="C88" s="19">
         <v>13</v>
       </c>
@@ -4183,10 +4663,10 @@
       </c>
     </row>
     <row r="89" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="37">
+      <c r="A89" s="38">
         <v>13</v>
       </c>
-      <c r="B89" s="38" t="s">
+      <c r="B89" s="39" t="s">
         <v>91</v>
       </c>
       <c r="C89" s="14">
@@ -4200,8 +4680,8 @@
       </c>
     </row>
     <row r="90" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="37"/>
-      <c r="B90" s="38"/>
+      <c r="A90" s="38"/>
+      <c r="B90" s="39"/>
       <c r="C90" s="14">
         <v>2</v>
       </c>
@@ -4213,8 +4693,8 @@
       </c>
     </row>
     <row r="91" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="37"/>
-      <c r="B91" s="38"/>
+      <c r="A91" s="38"/>
+      <c r="B91" s="39"/>
       <c r="C91" s="14">
         <v>3</v>
       </c>
@@ -4226,8 +4706,8 @@
       </c>
     </row>
     <row r="92" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="37"/>
-      <c r="B92" s="38"/>
+      <c r="A92" s="38"/>
+      <c r="B92" s="39"/>
       <c r="C92" s="14">
         <v>4</v>
       </c>
@@ -4239,8 +4719,8 @@
       </c>
     </row>
     <row r="93" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="37"/>
-      <c r="B93" s="38"/>
+      <c r="A93" s="38"/>
+      <c r="B93" s="39"/>
       <c r="C93" s="14">
         <v>5</v>
       </c>
@@ -4252,8 +4732,8 @@
       </c>
     </row>
     <row r="94" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="37"/>
-      <c r="B94" s="38"/>
+      <c r="A94" s="38"/>
+      <c r="B94" s="39"/>
       <c r="C94" s="14">
         <v>6</v>
       </c>
@@ -4265,8 +4745,8 @@
       </c>
     </row>
     <row r="95" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="37"/>
-      <c r="B95" s="38"/>
+      <c r="A95" s="38"/>
+      <c r="B95" s="39"/>
       <c r="C95" s="14">
         <v>7</v>
       </c>
@@ -4278,8 +4758,8 @@
       </c>
     </row>
     <row r="96" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="37"/>
-      <c r="B96" s="38"/>
+      <c r="A96" s="38"/>
+      <c r="B96" s="39"/>
       <c r="C96" s="14">
         <v>8</v>
       </c>
@@ -4291,8 +4771,8 @@
       </c>
     </row>
     <row r="97" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="37"/>
-      <c r="B97" s="38"/>
+      <c r="A97" s="38"/>
+      <c r="B97" s="39"/>
       <c r="C97" s="14">
         <v>9</v>
       </c>
@@ -4304,8 +4784,8 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="37"/>
-      <c r="B98" s="38"/>
+      <c r="A98" s="38"/>
+      <c r="B98" s="39"/>
       <c r="C98" s="14">
         <v>10</v>
       </c>
@@ -4317,8 +4797,8 @@
       </c>
     </row>
     <row r="99" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="37"/>
-      <c r="B99" s="38"/>
+      <c r="A99" s="38"/>
+      <c r="B99" s="39"/>
       <c r="C99" s="14">
         <v>11</v>
       </c>
@@ -4330,8 +4810,8 @@
       </c>
     </row>
     <row r="100" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="37"/>
-      <c r="B100" s="38"/>
+      <c r="A100" s="38"/>
+      <c r="B100" s="39"/>
       <c r="C100" s="14">
         <v>12</v>
       </c>
@@ -4343,8 +4823,8 @@
       </c>
     </row>
     <row r="101" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="37"/>
-      <c r="B101" s="38"/>
+      <c r="A101" s="38"/>
+      <c r="B101" s="39"/>
       <c r="C101" s="14">
         <v>13</v>
       </c>
@@ -4356,10 +4836,10 @@
       </c>
     </row>
     <row r="102" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="36">
+      <c r="A102" s="37">
         <v>12</v>
       </c>
-      <c r="B102" s="32" t="s">
+      <c r="B102" s="33" t="s">
         <v>100</v>
       </c>
       <c r="C102" s="19">
@@ -4373,8 +4853,8 @@
       </c>
     </row>
     <row r="103" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="36"/>
-      <c r="B103" s="32"/>
+      <c r="A103" s="37"/>
+      <c r="B103" s="33"/>
       <c r="C103" s="19">
         <v>2</v>
       </c>
@@ -4386,8 +4866,8 @@
       </c>
     </row>
     <row r="104" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="36"/>
-      <c r="B104" s="32"/>
+      <c r="A104" s="37"/>
+      <c r="B104" s="33"/>
       <c r="C104" s="19">
         <v>3</v>
       </c>
@@ -4399,8 +4879,8 @@
       </c>
     </row>
     <row r="105" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="36"/>
-      <c r="B105" s="32"/>
+      <c r="A105" s="37"/>
+      <c r="B105" s="33"/>
       <c r="C105" s="19">
         <v>4</v>
       </c>
@@ -4412,8 +4892,8 @@
       </c>
     </row>
     <row r="106" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="36"/>
-      <c r="B106" s="32"/>
+      <c r="A106" s="37"/>
+      <c r="B106" s="33"/>
       <c r="C106" s="19">
         <v>5</v>
       </c>
@@ -4425,8 +4905,8 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="36"/>
-      <c r="B107" s="32"/>
+      <c r="A107" s="37"/>
+      <c r="B107" s="33"/>
       <c r="C107" s="19">
         <v>6</v>
       </c>
@@ -4438,8 +4918,8 @@
       </c>
     </row>
     <row r="108" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="36"/>
-      <c r="B108" s="32"/>
+      <c r="A108" s="37"/>
+      <c r="B108" s="33"/>
       <c r="C108" s="19">
         <v>7</v>
       </c>
@@ -4451,8 +4931,8 @@
       </c>
     </row>
     <row r="109" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="36"/>
-      <c r="B109" s="32"/>
+      <c r="A109" s="37"/>
+      <c r="B109" s="33"/>
       <c r="C109" s="19">
         <v>8</v>
       </c>
@@ -4464,8 +4944,8 @@
       </c>
     </row>
     <row r="110" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="36"/>
-      <c r="B110" s="32"/>
+      <c r="A110" s="37"/>
+      <c r="B110" s="33"/>
       <c r="C110" s="19">
         <v>9</v>
       </c>
@@ -4477,8 +4957,8 @@
       </c>
     </row>
     <row r="111" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="36"/>
-      <c r="B111" s="32"/>
+      <c r="A111" s="37"/>
+      <c r="B111" s="33"/>
       <c r="C111" s="19">
         <v>10</v>
       </c>
@@ -4490,8 +4970,8 @@
       </c>
     </row>
     <row r="112" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="36"/>
-      <c r="B112" s="32"/>
+      <c r="A112" s="37"/>
+      <c r="B112" s="33"/>
       <c r="C112" s="19">
         <v>11</v>
       </c>
@@ -4503,8 +4983,8 @@
       </c>
     </row>
     <row r="113" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="36"/>
-      <c r="B113" s="32"/>
+      <c r="A113" s="37"/>
+      <c r="B113" s="33"/>
       <c r="C113" s="19">
         <v>12</v>
       </c>
@@ -4516,10 +4996,10 @@
       </c>
     </row>
     <row r="114" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="30">
+      <c r="A114" s="31">
         <v>14</v>
       </c>
-      <c r="B114" s="35" t="s">
+      <c r="B114" s="36" t="s">
         <v>113</v>
       </c>
       <c r="C114" s="24">
@@ -4533,8 +5013,8 @@
       </c>
     </row>
     <row r="115" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="30"/>
-      <c r="B115" s="35"/>
+      <c r="A115" s="31"/>
+      <c r="B115" s="36"/>
       <c r="C115" s="24">
         <v>2</v>
       </c>
@@ -4546,8 +5026,8 @@
       </c>
     </row>
     <row r="116" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="30"/>
-      <c r="B116" s="35"/>
+      <c r="A116" s="31"/>
+      <c r="B116" s="36"/>
       <c r="C116" s="24">
         <v>3</v>
       </c>
@@ -4559,8 +5039,8 @@
       </c>
     </row>
     <row r="117" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="30"/>
-      <c r="B117" s="35"/>
+      <c r="A117" s="31"/>
+      <c r="B117" s="36"/>
       <c r="C117" s="24">
         <v>4</v>
       </c>
@@ -4572,8 +5052,8 @@
       </c>
     </row>
     <row r="118" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="30"/>
-      <c r="B118" s="35"/>
+      <c r="A118" s="31"/>
+      <c r="B118" s="36"/>
       <c r="C118" s="24">
         <v>5</v>
       </c>
@@ -4585,8 +5065,8 @@
       </c>
     </row>
     <row r="119" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="30"/>
-      <c r="B119" s="35"/>
+      <c r="A119" s="31"/>
+      <c r="B119" s="36"/>
       <c r="C119" s="24">
         <v>6</v>
       </c>
@@ -4599,7 +5079,7 @@
     </row>
     <row r="120" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="6"/>
-      <c r="B120" s="35"/>
+      <c r="B120" s="36"/>
       <c r="C120" s="24">
         <v>7</v>
       </c>
@@ -4611,8 +5091,8 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="30"/>
-      <c r="B121" s="35"/>
+      <c r="A121" s="31"/>
+      <c r="B121" s="36"/>
       <c r="C121" s="24">
         <v>8</v>
       </c>
@@ -4624,8 +5104,8 @@
       </c>
     </row>
     <row r="122" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="30"/>
-      <c r="B122" s="35"/>
+      <c r="A122" s="31"/>
+      <c r="B122" s="36"/>
       <c r="C122" s="24">
         <v>9</v>
       </c>
@@ -4637,8 +5117,8 @@
       </c>
     </row>
     <row r="123" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="30"/>
-      <c r="B123" s="35"/>
+      <c r="A123" s="31"/>
+      <c r="B123" s="36"/>
       <c r="C123" s="24">
         <v>10</v>
       </c>
@@ -4650,8 +5130,8 @@
       </c>
     </row>
     <row r="124" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="30"/>
-      <c r="B124" s="35"/>
+      <c r="A124" s="31"/>
+      <c r="B124" s="36"/>
       <c r="C124" s="24">
         <v>11</v>
       </c>
@@ -4663,8 +5143,8 @@
       </c>
     </row>
     <row r="125" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="30"/>
-      <c r="B125" s="35"/>
+      <c r="A125" s="31"/>
+      <c r="B125" s="36"/>
       <c r="C125" s="24">
         <v>12</v>
       </c>
@@ -4676,8 +5156,8 @@
       </c>
     </row>
     <row r="126" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="30"/>
-      <c r="B126" s="32" t="s">
+      <c r="A126" s="31"/>
+      <c r="B126" s="33" t="s">
         <v>119</v>
       </c>
       <c r="C126" s="19">
@@ -4691,8 +5171,8 @@
       </c>
     </row>
     <row r="127" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="30"/>
-      <c r="B127" s="32"/>
+      <c r="A127" s="31"/>
+      <c r="B127" s="33"/>
       <c r="C127" s="19">
         <v>2</v>
       </c>
@@ -4704,8 +5184,8 @@
       </c>
     </row>
     <row r="128" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="30"/>
-      <c r="B128" s="32"/>
+      <c r="A128" s="31"/>
+      <c r="B128" s="33"/>
       <c r="C128" s="19">
         <v>3</v>
       </c>
@@ -4717,8 +5197,8 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="30"/>
-      <c r="B129" s="32"/>
+      <c r="A129" s="31"/>
+      <c r="B129" s="33"/>
       <c r="C129" s="19">
         <v>4</v>
       </c>
@@ -4730,8 +5210,8 @@
       </c>
     </row>
     <row r="130" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="30"/>
-      <c r="B130" s="32"/>
+      <c r="A130" s="31"/>
+      <c r="B130" s="33"/>
       <c r="C130" s="19">
         <v>5</v>
       </c>
@@ -4743,8 +5223,8 @@
       </c>
     </row>
     <row r="131" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="30"/>
-      <c r="B131" s="32"/>
+      <c r="A131" s="31"/>
+      <c r="B131" s="33"/>
       <c r="C131" s="19">
         <v>6</v>
       </c>
@@ -4756,10 +5236,10 @@
       </c>
     </row>
     <row r="132" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="30">
+      <c r="A132" s="31">
         <v>16</v>
       </c>
-      <c r="B132" s="34" t="s">
+      <c r="B132" s="35" t="s">
         <v>126</v>
       </c>
       <c r="C132" s="6">
@@ -4773,8 +5253,8 @@
       </c>
     </row>
     <row r="133" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="30"/>
-      <c r="B133" s="34"/>
+      <c r="A133" s="31"/>
+      <c r="B133" s="35"/>
       <c r="C133" s="6">
         <v>2</v>
       </c>
@@ -4786,8 +5266,8 @@
       </c>
     </row>
     <row r="134" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="30"/>
-      <c r="B134" s="34"/>
+      <c r="A134" s="31"/>
+      <c r="B134" s="35"/>
       <c r="C134" s="6">
         <v>3</v>
       </c>
@@ -4799,8 +5279,8 @@
       </c>
     </row>
     <row r="135" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="30"/>
-      <c r="B135" s="34"/>
+      <c r="A135" s="31"/>
+      <c r="B135" s="35"/>
       <c r="C135" s="6">
         <v>4</v>
       </c>
@@ -4812,8 +5292,8 @@
       </c>
     </row>
     <row r="136" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="30"/>
-      <c r="B136" s="34"/>
+      <c r="A136" s="31"/>
+      <c r="B136" s="35"/>
       <c r="C136" s="6">
         <v>5</v>
       </c>
@@ -4825,8 +5305,8 @@
       </c>
     </row>
     <row r="137" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="30"/>
-      <c r="B137" s="34"/>
+      <c r="A137" s="31"/>
+      <c r="B137" s="35"/>
       <c r="C137" s="6">
         <v>6</v>
       </c>
@@ -4838,10 +5318,10 @@
       </c>
     </row>
     <row r="138" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="30">
+      <c r="A138" s="31">
         <v>17</v>
       </c>
-      <c r="B138" s="31" t="s">
+      <c r="B138" s="32" t="s">
         <v>129</v>
       </c>
       <c r="C138" s="19">
@@ -4855,8 +5335,8 @@
       </c>
     </row>
     <row r="139" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="30"/>
-      <c r="B139" s="32"/>
+      <c r="A139" s="31"/>
+      <c r="B139" s="33"/>
       <c r="C139" s="19">
         <v>2</v>
       </c>
@@ -4868,8 +5348,8 @@
       </c>
     </row>
     <row r="140" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="30"/>
-      <c r="B140" s="32"/>
+      <c r="A140" s="31"/>
+      <c r="B140" s="33"/>
       <c r="C140" s="19">
         <v>3</v>
       </c>
@@ -4881,8 +5361,8 @@
       </c>
     </row>
     <row r="141" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="30"/>
-      <c r="B141" s="32"/>
+      <c r="A141" s="31"/>
+      <c r="B141" s="33"/>
       <c r="C141" s="19">
         <v>4</v>
       </c>
@@ -4894,8 +5374,8 @@
       </c>
     </row>
     <row r="142" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="30"/>
-      <c r="B142" s="32"/>
+      <c r="A142" s="31"/>
+      <c r="B142" s="33"/>
       <c r="C142" s="19">
         <v>5</v>
       </c>
@@ -4907,8 +5387,8 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="30"/>
-      <c r="B143" s="32"/>
+      <c r="A143" s="31"/>
+      <c r="B143" s="33"/>
       <c r="C143" s="19">
         <v>6</v>
       </c>
@@ -4920,8 +5400,8 @@
       </c>
     </row>
     <row r="144" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="30"/>
-      <c r="B144" s="32"/>
+      <c r="A144" s="31"/>
+      <c r="B144" s="33"/>
       <c r="C144" s="19">
         <v>7</v>
       </c>
@@ -4933,8 +5413,8 @@
       </c>
     </row>
     <row r="145" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="30"/>
-      <c r="B145" s="32"/>
+      <c r="A145" s="31"/>
+      <c r="B145" s="33"/>
       <c r="C145" s="19">
         <v>8</v>
       </c>
@@ -4946,10 +5426,10 @@
       </c>
     </row>
     <row r="146" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="30">
+      <c r="A146" s="31">
         <v>18</v>
       </c>
-      <c r="B146" s="33" t="s">
+      <c r="B146" s="34" t="s">
         <v>134</v>
       </c>
       <c r="C146" s="6">
@@ -4963,8 +5443,8 @@
       </c>
     </row>
     <row r="147" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="30"/>
-      <c r="B147" s="34"/>
+      <c r="A147" s="31"/>
+      <c r="B147" s="35"/>
       <c r="C147" s="6">
         <v>2</v>
       </c>
@@ -4976,8 +5456,8 @@
       </c>
     </row>
     <row r="148" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="30"/>
-      <c r="B148" s="34"/>
+      <c r="A148" s="31"/>
+      <c r="B148" s="35"/>
       <c r="C148" s="6">
         <v>3</v>
       </c>
@@ -4989,8 +5469,8 @@
       </c>
     </row>
     <row r="149" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="30"/>
-      <c r="B149" s="34"/>
+      <c r="A149" s="31"/>
+      <c r="B149" s="35"/>
       <c r="C149" s="6">
         <v>4</v>
       </c>
@@ -5002,8 +5482,8 @@
       </c>
     </row>
     <row r="150" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="30"/>
-      <c r="B150" s="34"/>
+      <c r="A150" s="31"/>
+      <c r="B150" s="35"/>
       <c r="C150" s="6">
         <v>5</v>
       </c>
@@ -5015,10 +5495,10 @@
       </c>
     </row>
     <row r="151" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="30">
+      <c r="A151" s="31">
         <v>19</v>
       </c>
-      <c r="B151" s="31" t="s">
+      <c r="B151" s="32" t="s">
         <v>139</v>
       </c>
       <c r="C151" s="19">
@@ -5032,8 +5512,8 @@
       </c>
     </row>
     <row r="152" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="30"/>
-      <c r="B152" s="32"/>
+      <c r="A152" s="31"/>
+      <c r="B152" s="33"/>
       <c r="C152" s="19">
         <v>2</v>
       </c>
@@ -5045,8 +5525,8 @@
       </c>
     </row>
     <row r="153" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="30"/>
-      <c r="B153" s="32"/>
+      <c r="A153" s="31"/>
+      <c r="B153" s="33"/>
       <c r="C153" s="19">
         <v>3</v>
       </c>
@@ -5058,8 +5538,8 @@
       </c>
     </row>
     <row r="154" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="30"/>
-      <c r="B154" s="32"/>
+      <c r="A154" s="31"/>
+      <c r="B154" s="33"/>
       <c r="C154" s="19">
         <v>4</v>
       </c>
@@ -5071,8 +5551,8 @@
       </c>
     </row>
     <row r="155" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="30"/>
-      <c r="B155" s="32"/>
+      <c r="A155" s="31"/>
+      <c r="B155" s="33"/>
       <c r="C155" s="19">
         <v>5</v>
       </c>
@@ -5109,199 +5589,199 @@
     </row>
     <row r="162" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="2"/>
-      <c r="E162" s="28"/>
+      <c r="E162" s="29"/>
     </row>
     <row r="163" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="2"/>
-      <c r="E163" s="28"/>
+      <c r="E163" s="29"/>
     </row>
     <row r="164" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2"/>
-      <c r="E164" s="28"/>
+      <c r="E164" s="29"/>
     </row>
     <row r="165" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="2"/>
-      <c r="E165" s="28"/>
+      <c r="E165" s="29"/>
     </row>
     <row r="166" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="2"/>
-      <c r="E166" s="28"/>
+      <c r="E166" s="29"/>
     </row>
     <row r="167" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="2"/>
-      <c r="E167" s="28"/>
+      <c r="E167" s="29"/>
     </row>
     <row r="168" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="2"/>
-      <c r="E168" s="28"/>
+      <c r="E168" s="29"/>
     </row>
     <row r="169" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="2"/>
-      <c r="E169" s="28"/>
+      <c r="E169" s="29"/>
     </row>
     <row r="170" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="2"/>
-      <c r="E170" s="28"/>
+      <c r="E170" s="29"/>
     </row>
     <row r="171" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="2"/>
-      <c r="E171" s="28"/>
+      <c r="E171" s="29"/>
     </row>
     <row r="172" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="2"/>
-      <c r="E172" s="28"/>
+      <c r="E172" s="29"/>
     </row>
     <row r="173" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="2"/>
-      <c r="E173" s="29"/>
+      <c r="E173" s="30"/>
     </row>
     <row r="174" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="2"/>
-      <c r="E174" s="29"/>
+      <c r="E174" s="30"/>
     </row>
     <row r="175" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="2"/>
-      <c r="E175" s="29"/>
+      <c r="E175" s="30"/>
     </row>
     <row r="176" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="2"/>
-      <c r="E176" s="29"/>
+      <c r="E176" s="30"/>
     </row>
     <row r="177" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="2"/>
-      <c r="E177" s="29"/>
+      <c r="E177" s="30"/>
     </row>
     <row r="178" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="2"/>
-      <c r="E178" s="29"/>
+      <c r="E178" s="30"/>
     </row>
     <row r="179" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="2"/>
-      <c r="E179" s="29"/>
+      <c r="E179" s="30"/>
     </row>
     <row r="180" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="2"/>
-      <c r="E180" s="29"/>
+      <c r="E180" s="30"/>
     </row>
     <row r="181" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="2"/>
-      <c r="E181" s="29"/>
+      <c r="E181" s="30"/>
     </row>
     <row r="182" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="2"/>
-      <c r="E182" s="29"/>
+      <c r="E182" s="30"/>
     </row>
     <row r="183" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="2"/>
-      <c r="E183" s="29"/>
+      <c r="E183" s="30"/>
     </row>
     <row r="184" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="2"/>
-      <c r="E184" s="29"/>
+      <c r="E184" s="30"/>
     </row>
     <row r="185" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="2"/>
-      <c r="E185" s="29"/>
+      <c r="E185" s="30"/>
     </row>
     <row r="186" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="2"/>
-      <c r="E186" s="29"/>
+      <c r="E186" s="30"/>
     </row>
     <row r="187" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="2"/>
-      <c r="E187" s="29"/>
+      <c r="E187" s="30"/>
     </row>
     <row r="188" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="2"/>
-      <c r="E188" s="29"/>
+      <c r="E188" s="30"/>
     </row>
     <row r="189" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="2"/>
-      <c r="E189" s="29"/>
+      <c r="E189" s="30"/>
     </row>
     <row r="190" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="2"/>
-      <c r="E190" s="29"/>
+      <c r="E190" s="30"/>
     </row>
     <row r="191" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="2"/>
-      <c r="E191" s="29"/>
+      <c r="E191" s="30"/>
     </row>
     <row r="192" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="2"/>
-      <c r="E192" s="29"/>
+      <c r="E192" s="30"/>
     </row>
     <row r="193" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="2"/>
-      <c r="E193" s="29"/>
+      <c r="E193" s="30"/>
     </row>
     <row r="194" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="2"/>
-      <c r="E194" s="29"/>
+      <c r="E194" s="30"/>
     </row>
     <row r="195" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="2"/>
-      <c r="E195" s="29"/>
+      <c r="E195" s="30"/>
     </row>
     <row r="196" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="2"/>
-      <c r="E196" s="29"/>
+      <c r="E196" s="30"/>
     </row>
     <row r="197" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="2"/>
-      <c r="E197" s="29"/>
+      <c r="E197" s="30"/>
     </row>
     <row r="198" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="2"/>
-      <c r="E198" s="28"/>
+      <c r="E198" s="29"/>
     </row>
     <row r="199" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="2"/>
-      <c r="E199" s="28"/>
+      <c r="E199" s="29"/>
     </row>
     <row r="200" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="2"/>
-      <c r="E200" s="28"/>
+      <c r="E200" s="29"/>
     </row>
     <row r="201" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="2"/>
-      <c r="E201" s="28"/>
+      <c r="E201" s="29"/>
     </row>
     <row r="202" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="2"/>
-      <c r="E202" s="28"/>
+      <c r="E202" s="29"/>
     </row>
     <row r="203" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="2"/>
-      <c r="E203" s="28"/>
+      <c r="E203" s="29"/>
     </row>
     <row r="204" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="2"/>
-      <c r="E204" s="28"/>
+      <c r="E204" s="29"/>
     </row>
     <row r="205" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="2"/>
-      <c r="E205" s="28"/>
+      <c r="E205" s="29"/>
     </row>
     <row r="206" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="2"/>
-      <c r="E206" s="28"/>
+      <c r="E206" s="29"/>
     </row>
     <row r="207" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="2"/>
-      <c r="E207" s="28"/>
+      <c r="E207" s="29"/>
     </row>
     <row r="208" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="2"/>
-      <c r="E208" s="28"/>
+      <c r="E208" s="29"/>
     </row>
     <row r="209" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="2"/>
-      <c r="E209" s="28"/>
+      <c r="E209" s="29"/>
     </row>
     <row r="210" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="2"/>
-      <c r="E210" s="28"/>
+      <c r="E210" s="29"/>
     </row>
     <row r="211" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="2"/>
@@ -9092,8 +9572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView zoomScale="80" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9105,32 +9585,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="47" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="30">
+      <c r="A3" s="31">
         <v>1</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="6">
@@ -9144,8 +9624,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="30"/>
-      <c r="B4" s="29"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="6">
         <v>2</v>
       </c>
@@ -9157,8 +9637,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
-      <c r="B5" s="29"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="6">
         <v>3</v>
       </c>
@@ -9170,8 +9650,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
-      <c r="B6" s="29"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="6">
         <v>4</v>
       </c>
@@ -9183,8 +9663,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
-      <c r="B7" s="29"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="6">
         <v>5</v>
       </c>
@@ -9196,10 +9676,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="30">
+      <c r="A8" s="31">
         <v>2</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="30" t="s">
         <v>142</v>
       </c>
       <c r="C8" s="6">
@@ -9213,8 +9693,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
-      <c r="B9" s="29"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="6">
         <v>2</v>
       </c>
@@ -9226,8 +9706,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
-      <c r="B10" s="29"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="6">
         <v>3</v>
       </c>
@@ -9239,8 +9719,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
-      <c r="B11" s="29"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="6">
         <v>4</v>
       </c>
@@ -9252,10 +9732,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="30">
+      <c r="A12" s="31">
         <v>3</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="30" t="s">
         <v>146</v>
       </c>
       <c r="C12" s="6">
@@ -9269,8 +9749,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="30"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="6">
         <v>2</v>
       </c>
@@ -9282,8 +9762,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="30"/>
-      <c r="B14" s="29"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="6">
         <v>3</v>
       </c>
@@ -9295,8 +9775,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="30"/>
-      <c r="B15" s="29"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="6">
         <v>4</v>
       </c>
@@ -9308,10 +9788,10 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="30">
+      <c r="A16" s="31">
         <v>4</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="30" t="s">
         <v>151</v>
       </c>
       <c r="C16" s="6">
@@ -9325,8 +9805,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="30"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="6">
         <v>2</v>
       </c>
@@ -9338,8 +9818,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="6">
         <v>3</v>
       </c>
@@ -9351,8 +9831,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="30"/>
-      <c r="B19" s="29"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="6">
         <v>4</v>
       </c>
@@ -9364,8 +9844,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="30"/>
-      <c r="B20" s="29"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="6">
         <v>5</v>
       </c>
@@ -9377,10 +9857,10 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="30">
+      <c r="A21" s="31">
         <v>5</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="30" t="s">
         <v>157</v>
       </c>
       <c r="C21" s="6">
@@ -9394,8 +9874,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="30"/>
-      <c r="B22" s="29"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="6">
         <v>2</v>
       </c>
@@ -9407,8 +9887,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="30"/>
-      <c r="B23" s="29"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="6">
         <v>3</v>
       </c>
@@ -9420,8 +9900,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="30"/>
-      <c r="B24" s="29"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="6">
         <v>4</v>
       </c>
@@ -9433,8 +9913,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="30"/>
-      <c r="B25" s="29"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="6">
         <v>5</v>
       </c>
@@ -9446,16 +9926,16 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="30">
-        <v>5</v>
-      </c>
-      <c r="B26" s="29" t="s">
+      <c r="A26" s="31">
+        <v>6</v>
+      </c>
+      <c r="B26" s="30" t="s">
         <v>163</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
       </c>
-      <c r="D26" s="51" t="s">
+      <c r="D26" s="28" t="s">
         <v>164</v>
       </c>
       <c r="E26" s="7" t="s">
@@ -9463,12 +9943,12 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="30"/>
-      <c r="B27" s="29"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="6">
         <v>2</v>
       </c>
-      <c r="D27" s="51" t="s">
+      <c r="D27" s="28" t="s">
         <v>165</v>
       </c>
       <c r="E27" s="11" t="s">
@@ -9476,12 +9956,12 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="50"/>
-      <c r="B28" s="29"/>
+      <c r="A28" s="49"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="6">
         <v>3</v>
       </c>
-      <c r="D28" s="51" t="s">
+      <c r="D28" s="28" t="s">
         <v>166</v>
       </c>
       <c r="E28" s="11" t="s">
@@ -9489,12 +9969,12 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="50"/>
-      <c r="B29" s="29"/>
+      <c r="A29" s="49"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="6">
         <v>4</v>
       </c>
-      <c r="D29" s="51" t="s">
+      <c r="D29" s="28" t="s">
         <v>167</v>
       </c>
       <c r="E29" s="11" t="s">
@@ -9502,12 +9982,12 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="50"/>
-      <c r="B30" s="29"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="6">
         <v>5</v>
       </c>
-      <c r="D30" s="51" t="s">
+      <c r="D30" s="28" t="s">
         <v>168</v>
       </c>
       <c r="E30" s="11" t="s">
@@ -9515,12 +9995,12 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="50"/>
-      <c r="B31" s="29"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="6">
         <v>6</v>
       </c>
-      <c r="D31" s="51" t="s">
+      <c r="D31" s="28" t="s">
         <v>169</v>
       </c>
       <c r="E31" s="11" t="s">
@@ -9528,12 +10008,12 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="50"/>
-      <c r="B32" s="29"/>
+      <c r="A32" s="49"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="6">
         <v>7</v>
       </c>
-      <c r="D32" s="51" t="s">
+      <c r="D32" s="28" t="s">
         <v>170</v>
       </c>
       <c r="E32" s="11" t="s">
@@ -9541,12 +10021,12 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="50"/>
-      <c r="B33" s="29"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="6">
         <v>8</v>
       </c>
-      <c r="D33" s="51" t="s">
+      <c r="D33" s="28" t="s">
         <v>171</v>
       </c>
       <c r="E33" s="11" t="s">
@@ -9582,4 +10062,709 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5EFADB-3276-4FDB-BFC6-0820002A2F15}">
+  <dimension ref="A1:E50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" customWidth="1"/>
+    <col min="4" max="4" width="233.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="46"/>
+      <c r="E2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="31">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="49"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="49"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="6">
+        <v>3</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="49"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="49"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="6">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="31"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="6">
+        <v>6</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>195</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="31"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="6">
+        <v>7</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="49"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="6">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="49"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="6">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="31"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="6">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="31"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="6">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="31">
+        <v>2</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="49"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="6">
+        <v>2</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="49"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="6">
+        <v>3</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="49"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="6">
+        <v>4</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="49"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="6">
+        <v>5</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="49"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="6">
+        <v>6</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="49"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="6">
+        <v>7</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="49"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="6">
+        <v>8</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="49"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="6">
+        <v>9</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="49"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="6">
+        <v>10</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="49"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="6">
+        <v>11</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="49"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="6">
+        <v>12</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="31">
+        <v>3</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1</v>
+      </c>
+      <c r="D26" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="31"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="6">
+        <v>2</v>
+      </c>
+      <c r="D27" s="52" t="s">
+        <v>184</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="31"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="6">
+        <v>3</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="31"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="6">
+        <v>4</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="31"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="6">
+        <v>5</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="31">
+        <v>4</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="C31" s="6">
+        <v>1</v>
+      </c>
+      <c r="D31" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="31"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="6">
+        <v>2</v>
+      </c>
+      <c r="D32" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="31"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="6">
+        <v>3</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="31"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="6">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="31"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="6">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="31">
+        <v>5</v>
+      </c>
+      <c r="B36" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="C36" s="6">
+        <v>1</v>
+      </c>
+      <c r="D36" s="52" t="s">
+        <v>181</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="31"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="6">
+        <v>2</v>
+      </c>
+      <c r="D37" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="31"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="6">
+        <v>3</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="31"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="6">
+        <v>4</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="31"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="6">
+        <v>5</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="31">
+        <v>6</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="C41" s="6">
+        <v>1</v>
+      </c>
+      <c r="D41" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="31"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="6">
+        <v>2</v>
+      </c>
+      <c r="D42" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="31"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="6">
+        <v>3</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="31"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="6">
+        <v>4</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="31"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="6">
+        <v>5</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="31">
+        <v>7</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="C46" s="6">
+        <v>1</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="31"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="6">
+        <v>2</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="31"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="6">
+        <v>3</v>
+      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="31"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="6">
+        <v>4</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="31"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="6">
+        <v>5</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A30"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>